<commit_message>
Perbaikan template xlsx mass upload project
</commit_message>
<xml_diff>
--- a/dashboard/static/dashboard/sample/project_upload_template.xlsx
+++ b/dashboard/static/dashboard/sample/project_upload_template.xlsx
@@ -1,33 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO LOQ\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PORTOFOLIO ADIT\DJANGO AHSP PROJECT\dashboard\static\dashboard\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DC2ED0-B091-4AB2-9303-71CA5DD43DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF214B-B391-4E26-9FC5-0B56F190B23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <si>
     <t>nama</t>
   </si>
   <si>
-    <t>tahun_project</t>
-  </si>
-  <si>
     <t>sumber_dana</t>
   </si>
   <si>
@@ -74,13 +84,502 @@
   </si>
   <si>
     <t>kategori</t>
+  </si>
+  <si>
+    <t>tanggal_mulai</t>
+  </si>
+  <si>
+    <t>Pemilik 1</t>
+  </si>
+  <si>
+    <t>Lokasi 1</t>
+  </si>
+  <si>
+    <t>Client 1</t>
+  </si>
+  <si>
+    <t>ket project satu 1</t>
+  </si>
+  <si>
+    <t>ket project dua 1</t>
+  </si>
+  <si>
+    <t>jabatan client 1</t>
+  </si>
+  <si>
+    <t>instansi client 1</t>
+  </si>
+  <si>
+    <t>kontraktor 1</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 1</t>
+  </si>
+  <si>
+    <t>konsultan perencana 1</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 1</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 1</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 1</t>
+  </si>
+  <si>
+    <t>deskripsi 1</t>
+  </si>
+  <si>
+    <t>kategori 1</t>
+  </si>
+  <si>
+    <t>Pemilik 2</t>
+  </si>
+  <si>
+    <t>Lokasi 2</t>
+  </si>
+  <si>
+    <t>Client 2</t>
+  </si>
+  <si>
+    <t>ket project satu 2</t>
+  </si>
+  <si>
+    <t>ket project dua 2</t>
+  </si>
+  <si>
+    <t>jabatan client 2</t>
+  </si>
+  <si>
+    <t>instansi client 2</t>
+  </si>
+  <si>
+    <t>kontraktor 2</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 2</t>
+  </si>
+  <si>
+    <t>konsultan perencana 2</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 2</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 2</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 2</t>
+  </si>
+  <si>
+    <t>deskripsi 2</t>
+  </si>
+  <si>
+    <t>kategori 2</t>
+  </si>
+  <si>
+    <t>Pemilik 3</t>
+  </si>
+  <si>
+    <t>Lokasi 3</t>
+  </si>
+  <si>
+    <t>Client 3</t>
+  </si>
+  <si>
+    <t>ket project satu 3</t>
+  </si>
+  <si>
+    <t>ket project dua 3</t>
+  </si>
+  <si>
+    <t>jabatan client 3</t>
+  </si>
+  <si>
+    <t>instansi client 3</t>
+  </si>
+  <si>
+    <t>kontraktor 3</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 3</t>
+  </si>
+  <si>
+    <t>konsultan perencana 3</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 3</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 3</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 3</t>
+  </si>
+  <si>
+    <t>deskripsi 3</t>
+  </si>
+  <si>
+    <t>kategori 3</t>
+  </si>
+  <si>
+    <t>Pemilik 4</t>
+  </si>
+  <si>
+    <t>Lokasi 4</t>
+  </si>
+  <si>
+    <t>Client 4</t>
+  </si>
+  <si>
+    <t>ket project satu 4</t>
+  </si>
+  <si>
+    <t>ket project dua 4</t>
+  </si>
+  <si>
+    <t>jabatan client 4</t>
+  </si>
+  <si>
+    <t>instansi client 4</t>
+  </si>
+  <si>
+    <t>kontraktor 4</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 4</t>
+  </si>
+  <si>
+    <t>konsultan perencana 4</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 4</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 4</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 4</t>
+  </si>
+  <si>
+    <t>deskripsi 4</t>
+  </si>
+  <si>
+    <t>kategori 4</t>
+  </si>
+  <si>
+    <t>Pemilik 5</t>
+  </si>
+  <si>
+    <t>Lokasi 5</t>
+  </si>
+  <si>
+    <t>Client 5</t>
+  </si>
+  <si>
+    <t>ket project satu 5</t>
+  </si>
+  <si>
+    <t>ket project dua 5</t>
+  </si>
+  <si>
+    <t>jabatan client 5</t>
+  </si>
+  <si>
+    <t>instansi client 5</t>
+  </si>
+  <si>
+    <t>kontraktor 5</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 5</t>
+  </si>
+  <si>
+    <t>konsultan perencana 5</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 5</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 5</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 5</t>
+  </si>
+  <si>
+    <t>deskripsi 5</t>
+  </si>
+  <si>
+    <t>kategori 5</t>
+  </si>
+  <si>
+    <t>Pemilik 6</t>
+  </si>
+  <si>
+    <t>Lokasi 6</t>
+  </si>
+  <si>
+    <t>Client 6</t>
+  </si>
+  <si>
+    <t>ket project satu 6</t>
+  </si>
+  <si>
+    <t>ket project dua 6</t>
+  </si>
+  <si>
+    <t>jabatan client 6</t>
+  </si>
+  <si>
+    <t>instansi client 6</t>
+  </si>
+  <si>
+    <t>kontraktor 6</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 6</t>
+  </si>
+  <si>
+    <t>konsultan perencana 6</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 6</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 6</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 6</t>
+  </si>
+  <si>
+    <t>deskripsi 6</t>
+  </si>
+  <si>
+    <t>kategori 6</t>
+  </si>
+  <si>
+    <t>tanggal_selesai</t>
+  </si>
+  <si>
+    <t>durasi_hari</t>
+  </si>
+  <si>
+    <t>Pemilik 7</t>
+  </si>
+  <si>
+    <t>Lokasi 7</t>
+  </si>
+  <si>
+    <t>Client 7</t>
+  </si>
+  <si>
+    <t>ket project satu 7</t>
+  </si>
+  <si>
+    <t>ket project dua 7</t>
+  </si>
+  <si>
+    <t>jabatan client 7</t>
+  </si>
+  <si>
+    <t>instansi client 7</t>
+  </si>
+  <si>
+    <t>kontraktor 7</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 7</t>
+  </si>
+  <si>
+    <t>konsultan perencana 7</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 7</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 7</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 7</t>
+  </si>
+  <si>
+    <t>deskripsi 7</t>
+  </si>
+  <si>
+    <t>kategori 7</t>
+  </si>
+  <si>
+    <t>Pemilik 8</t>
+  </si>
+  <si>
+    <t>Lokasi 8</t>
+  </si>
+  <si>
+    <t>Client 8</t>
+  </si>
+  <si>
+    <t>ket project satu 8</t>
+  </si>
+  <si>
+    <t>ket project dua 8</t>
+  </si>
+  <si>
+    <t>jabatan client 8</t>
+  </si>
+  <si>
+    <t>instansi client 8</t>
+  </si>
+  <si>
+    <t>kontraktor 8</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 8</t>
+  </si>
+  <si>
+    <t>konsultan perencana 8</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 8</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 8</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 8</t>
+  </si>
+  <si>
+    <t>deskripsi 8</t>
+  </si>
+  <si>
+    <t>kategori 8</t>
+  </si>
+  <si>
+    <t>Pemilik 9</t>
+  </si>
+  <si>
+    <t>Lokasi 9</t>
+  </si>
+  <si>
+    <t>Client 9</t>
+  </si>
+  <si>
+    <t>ket project satu 9</t>
+  </si>
+  <si>
+    <t>ket project dua 9</t>
+  </si>
+  <si>
+    <t>jabatan client 9</t>
+  </si>
+  <si>
+    <t>instansi client 9</t>
+  </si>
+  <si>
+    <t>kontraktor 9</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 9</t>
+  </si>
+  <si>
+    <t>konsultan perencana 9</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 9</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 9</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 9</t>
+  </si>
+  <si>
+    <t>deskripsi 9</t>
+  </si>
+  <si>
+    <t>kategori 9</t>
+  </si>
+  <si>
+    <t>Pemilik 10</t>
+  </si>
+  <si>
+    <t>Lokasi 10</t>
+  </si>
+  <si>
+    <t>Client 10</t>
+  </si>
+  <si>
+    <t>ket project satu 10</t>
+  </si>
+  <si>
+    <t>ket project dua 10</t>
+  </si>
+  <si>
+    <t>jabatan client 10</t>
+  </si>
+  <si>
+    <t>instansi client 10</t>
+  </si>
+  <si>
+    <t>kontraktor 10</t>
+  </si>
+  <si>
+    <t>instansi kontraktor 10</t>
+  </si>
+  <si>
+    <t>konsultan perencana 10</t>
+  </si>
+  <si>
+    <t>instansi konsultan perencana 10</t>
+  </si>
+  <si>
+    <t>konsultan pengawas 10</t>
+  </si>
+  <si>
+    <t>instansi konsultan pengawas 10</t>
+  </si>
+  <si>
+    <t>deskripsi 10</t>
+  </si>
+  <si>
+    <t>kategori 10</t>
+  </si>
+  <si>
+    <t>Project template test 1</t>
+  </si>
+  <si>
+    <t>Project template test 2</t>
+  </si>
+  <si>
+    <t>Project template test 3</t>
+  </si>
+  <si>
+    <t>Project template test 4</t>
+  </si>
+  <si>
+    <t>Project template test 5</t>
+  </si>
+  <si>
+    <t>Project template test 6</t>
+  </si>
+  <si>
+    <t>Project template test 7</t>
+  </si>
+  <si>
+    <t>Project template test 8</t>
+  </si>
+  <si>
+    <t>Project template test 9</t>
+  </si>
+  <si>
+    <t>Project template test 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +591,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,11 +637,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,76 +947,728 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="47.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2">
+        <v>46023</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>1000000001</v>
+      </c>
+      <c r="G2" s="2">
+        <v>46346</v>
+      </c>
+      <c r="H2">
+        <f>G2-B2</f>
+        <v>323</v>
+      </c>
+      <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="2">
+        <v>46024</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3">
+        <v>1000000002</v>
+      </c>
+      <c r="G3" s="2">
+        <v>46347</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H7" si="0">G3-B3</f>
+        <v>323</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="2">
+        <v>46025</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4">
+        <v>1000000003</v>
+      </c>
+      <c r="G4" s="2">
+        <v>46348</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+      <c r="I4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="2">
+        <v>46026</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5">
+        <v>1000000004</v>
+      </c>
+      <c r="G5" s="2">
+        <v>46349</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
+        <v>70</v>
+      </c>
+      <c r="N5" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+      <c r="P5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" t="s">
+        <v>75</v>
+      </c>
+      <c r="S5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="2">
+        <v>46027</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6">
+        <v>1000000005</v>
+      </c>
+      <c r="G6" s="2">
+        <v>46350</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+      <c r="I6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L6" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" t="s">
+        <v>85</v>
+      </c>
+      <c r="N6" t="s">
+        <v>86</v>
+      </c>
+      <c r="O6" t="s">
+        <v>87</v>
+      </c>
+      <c r="P6" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6" t="s">
+        <v>90</v>
+      </c>
+      <c r="S6" t="s">
+        <v>91</v>
+      </c>
+      <c r="T6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="2">
+        <v>46028</v>
+      </c>
+      <c r="C7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7">
+        <v>1000000006</v>
+      </c>
+      <c r="G7" s="2">
+        <v>46351</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>323</v>
+      </c>
+      <c r="I7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L7" t="s">
+        <v>99</v>
+      </c>
+      <c r="M7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N7" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" t="s">
+        <v>102</v>
+      </c>
+      <c r="P7" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>104</v>
+      </c>
+      <c r="R7" t="s">
+        <v>105</v>
+      </c>
+      <c r="S7" t="s">
+        <v>106</v>
+      </c>
+      <c r="T7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="2">
+        <v>46029</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8">
+        <v>1000000007</v>
+      </c>
+      <c r="G8" s="2">
+        <v>46352</v>
+      </c>
+      <c r="H8">
+        <f>G8-B8</f>
+        <v>323</v>
+      </c>
+      <c r="I8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" t="s">
+        <v>115</v>
+      </c>
+      <c r="L8" t="s">
+        <v>116</v>
+      </c>
+      <c r="M8" t="s">
+        <v>117</v>
+      </c>
+      <c r="N8" t="s">
+        <v>118</v>
+      </c>
+      <c r="O8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P8" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>121</v>
+      </c>
+      <c r="R8" t="s">
+        <v>122</v>
+      </c>
+      <c r="S8" t="s">
+        <v>123</v>
+      </c>
+      <c r="T8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="2">
+        <v>46030</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9">
+        <v>1000000008</v>
+      </c>
+      <c r="G9" s="2">
+        <v>46353</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H11" si="1">G9-B9</f>
+        <v>323</v>
+      </c>
+      <c r="I9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" t="s">
+        <v>131</v>
+      </c>
+      <c r="M9" t="s">
+        <v>132</v>
+      </c>
+      <c r="N9" t="s">
+        <v>133</v>
+      </c>
+      <c r="O9" t="s">
+        <v>134</v>
+      </c>
+      <c r="P9" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>136</v>
+      </c>
+      <c r="R9" t="s">
+        <v>137</v>
+      </c>
+      <c r="S9" t="s">
+        <v>138</v>
+      </c>
+      <c r="T9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="2">
+        <v>46031</v>
+      </c>
+      <c r="C10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10">
+        <v>1000000009</v>
+      </c>
+      <c r="G10" s="2">
+        <v>46354</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>323</v>
+      </c>
+      <c r="I10" t="s">
+        <v>143</v>
+      </c>
+      <c r="J10" t="s">
+        <v>144</v>
+      </c>
+      <c r="K10" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" t="s">
+        <v>146</v>
+      </c>
+      <c r="M10" t="s">
+        <v>147</v>
+      </c>
+      <c r="N10" t="s">
+        <v>148</v>
+      </c>
+      <c r="O10" t="s">
+        <v>149</v>
+      </c>
+      <c r="P10" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>151</v>
+      </c>
+      <c r="R10" t="s">
+        <v>152</v>
+      </c>
+      <c r="S10" t="s">
+        <v>153</v>
+      </c>
+      <c r="T10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="2">
+        <v>46032</v>
+      </c>
+      <c r="C11" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11">
+        <v>1000000010</v>
+      </c>
+      <c r="G11" s="2">
+        <v>46355</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>323</v>
+      </c>
+      <c r="I11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J11" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" t="s">
+        <v>161</v>
+      </c>
+      <c r="M11" t="s">
+        <v>162</v>
+      </c>
+      <c r="N11" t="s">
+        <v>163</v>
+      </c>
+      <c r="O11" t="s">
+        <v>164</v>
+      </c>
+      <c r="P11" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>166</v>
+      </c>
+      <c r="R11" t="s">
+        <v>167</v>
+      </c>
+      <c r="S11" t="s">
+        <v>168</v>
+      </c>
+      <c r="T11" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>